<commit_message>
(Fix) Benchmark tool: Allow to show percentages larger than 100% and increase progress height
</commit_message>
<xml_diff>
--- a/wiki/UVtools_Compression.xlsx
+++ b/wiki/UVtools_Compression.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiago\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8969c3c35c0f8657/Programming/C^N/UVtools/wiki/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4029DB8C-79AA-4EAD-A7CF-5977EB23ADDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{4029DB8C-79AA-4EAD-A7CF-5977EB23ADDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8115B492-FF36-4A7F-B4CD-2C28F5AC3A94}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{70AB337B-0F1B-4C89-A9AC-5CAB5ECA9F86}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{70AB337B-0F1B-4C89-A9AC-5CAB5ECA9F86}"/>
   </bookViews>
   <sheets>
-    <sheet name="Folha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Folha2" sheetId="2" r:id="rId1"/>
+    <sheet name="Folha1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>PNG</t>
   </si>
@@ -57,12 +57,33 @@
   <si>
     <t>Bytes</t>
   </si>
+  <si>
+    <t>Bitmap</t>
+  </si>
+  <si>
+    <t>CPU:</t>
+  </si>
+  <si>
+    <t>13th Gen Intel(R) Core(TM) i9-13900K</t>
+  </si>
+  <si>
+    <t>RAM:</t>
+  </si>
+  <si>
+    <t>G.Skill Trident Z5 32GB DDR5-6400MHz CL32</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>8K Bitmap:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +93,14 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -99,17 +128,58 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -165,7 +235,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="pt-PT"/>
-              <a:t>ayer compression</a:t>
+              <a:t>ayer compression perfomance</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -211,7 +281,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Folha1!$C$1</c:f>
+              <c:f>Folha1!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -232,7 +302,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Folha1!$B$2:$B$5</c:f>
+              <c:f>Folha1!$B$4:$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -252,21 +322,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Folha1!$C$2:$C$5</c:f>
+              <c:f>Folha1!$C$4:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>14.28</c:v>
+                  <c:v>22.17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45.77</c:v>
+                  <c:v>63.29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46.3</c:v>
+                  <c:v>64.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>148.15</c:v>
+                  <c:v>312.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -282,7 +352,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Folha1!$D$1</c:f>
+              <c:f>Folha1!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -303,7 +373,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Folha1!$B$2:$B$5</c:f>
+              <c:f>Folha1!$B$4:$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -323,21 +393,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Folha1!$D$2:$D$5</c:f>
+              <c:f>Folha1!$D$4:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>124.1</c:v>
+                  <c:v>369</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>397.47</c:v>
+                  <c:v>1020.41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>406.5</c:v>
+                  <c:v>1033.06</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>907.44</c:v>
+                  <c:v>6097.56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -676,6 +746,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Compressed Bytes</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -717,7 +812,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Folha1!$G$1</c:f>
+              <c:f>Folha1!$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -738,7 +833,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Folha1!$F$2:$F$5</c:f>
+              <c:f>Folha1!$F$4:$F$7</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -758,7 +853,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Folha1!$G$2:$G$5</c:f>
+              <c:f>Folha1!$G$4:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2040,14 +2135,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>42861</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>168658</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2076,14 +2171,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>61912</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>170793</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2108,7 +2203,91 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>9419</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>132278</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>104669</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>1045</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagem 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F0CCB18-2987-49F1-99A3-F1D69BD5CAD2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8640534" y="1275278"/>
+          <a:ext cx="8609135" cy="5393267"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AF52C079-5C8B-4275-B4B1-B22DEB64B4B1}" name="Tabela1" displayName="Tabela1" ref="B3:D7" totalsRowShown="0" headerRowDxfId="4" dataDxfId="5">
+  <autoFilter ref="B3:D7" xr:uid="{AF52C079-5C8B-4275-B4B1-B22DEB64B4B1}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{ABD84F52-17AA-4DEB-9C66-78F50A4474E3}" name="Algorithm" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{953474D9-F5FE-4B8A-A20E-FB628240EAE3}" name="Single-Thread" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{49D707C4-9595-46B1-B31B-76F36BE02788}" name="Multi-thread" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A84CB058-FF2A-4039-9F93-B5C2BBA5DF84}" name="Tabela2" displayName="Tabela2" ref="F3:G8" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="F3:G8" xr:uid="{A84CB058-FF2A-4039-9F93-B5C2BBA5DF84}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{D59C5F30-117F-47D7-ADB2-4F7A09D56C03}" name="Algorithm" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{F2652AFC-A737-4733-8DC5-F294CD1AA3A1}" name="Bytes" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2407,115 +2586,173 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F11AA2D-3DD5-4188-9E72-8FA651C1AA77}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAFAB150-2DCD-41BC-A97C-EA4F89126505}">
-  <dimension ref="B1:I27"/>
+  <dimension ref="B1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="4"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>14.28</v>
-      </c>
-      <c r="D2" s="1">
-        <v>124.1</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1170575</v>
-      </c>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>45.77</v>
-      </c>
-      <c r="D3" s="1">
-        <v>397.47</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1">
-        <v>680507</v>
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>46.3</v>
+        <v>22.17</v>
       </c>
       <c r="D4" s="1">
-        <v>406.5</v>
+        <v>369</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>680497</v>
+        <v>1170575</v>
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>148.15</v>
+        <v>63.29</v>
       </c>
       <c r="D5" s="1">
-        <v>907.44</v>
+        <v>1020.41</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1">
-        <v>496376</v>
+        <v>680507</v>
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="27" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I27" s="2"/>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1033.06</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>680497</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="K6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="7"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>312.5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6097.56</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1">
+        <v>496376</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="1">
+        <v>33177600</v>
+      </c>
+    </row>
+    <row r="29" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I29" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="F1:I1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <tableParts count="2">
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>